<commit_message>
Compile rc4.  Resolved Evap and Transp calculations in cohort library.
</commit_message>
<xml_diff>
--- a/deploy/docs/Soil_temp_calculations.xlsx
+++ b/deploy/docs/Soil_temp_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\aruzicka555\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A775B9A1-354E-4F42-89C5-9B572185FB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803D1D4-D276-4825-97AC-BEFE8F4E0BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29565" yWindow="-7560" windowWidth="14685" windowHeight="14460" xr2:uid="{B5CA6E75-4B5B-4C46-9481-06C855E228A5}"/>
+    <workbookView xWindow="46005" yWindow="-14220" windowWidth="27345" windowHeight="14370" xr2:uid="{B5CA6E75-4B5B-4C46-9481-06C855E228A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -259,6 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,7 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,6 +293,1100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Temp</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$8:$Z$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>-17.00484441249812</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-19.653194628042449</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-19.372334909694636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16.64175494242421</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-12.273176951774708</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.3202552866782762</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.3832117038219316</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2057837602874955</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6351590199703221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.8835579201980153E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.5253529493632865</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-11.053815004516446</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-13.878522650663767</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-14.835536336740057</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-15.038584042011522</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-13.341026622018919</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-10.138726960643753</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6.4380188326888526</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7313304593948766</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9860731600280639</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.3432756136563011</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-4.6821558043398168</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9.3622348903929691</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-12.997688535326821</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-14.419019321604416</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-14.940728439664976</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-13.328791322693094</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-10.221991319342143</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-6.6156957336758797</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-3.9701887941571483</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.2275777629489788</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.2606369235832293</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.78035644119023306</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-4.7972797297344254</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-9.4268461551629184</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-12.271059639315581</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-14.177187763744948</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-14.24919371744225</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-12.714879701320793</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-10.463351517901863</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-7.703932337651878</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-5.4357495933556335</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-6.6122951549214566</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.2150207276110425</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.0439507524222424</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-3.3304786547481999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-7.9560035802502878</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-12.277575704785537</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-15.566715023772886</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-19.289690681967105</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-19.817454940879045</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-17.260571242706892</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-13.370247099252412</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-9.7143354986101258</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-5.2966988264993455</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.5153076727786612E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.64905326870430713</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-1.5355216963355431</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-6.7635503122237211</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-11.782183026125237</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-16.289407928830634</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-18.091296657176922</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-18.483055200010259</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-16.88394658860447</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-13.535420942447086</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-10.157010569821558</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-6.952593303481768</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-0.79958565351010868</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-3.3655081831444633</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-8.0755273371996079</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-13.515461036540215</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-17.376210661868939</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-18.158592383685601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9636-4E82-A7CD-7EB35672565E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1942037104"/>
+        <c:axId val="1942034608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1942037104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1942034608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1942034608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1942037104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>118518</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>56062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>423318</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>86542</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12E1C40A-5556-4299-B067-23CE883968D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,34 +1688,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D402A71-BB82-47A0-B5BC-2169AB86B423}">
   <dimension ref="A2:Z91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="AE40" sqref="AE40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="5" max="7" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="F2" s="10" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -644,7 +1738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.45118429999999998</v>
       </c>
@@ -655,7 +1749,7 @@
         <v>0.8</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
         <f>(1 - $B$4) * 360 + $B$4 * 80</f>
@@ -670,42 +1764,42 @@
         <v>2954.4575691999999</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="I6" s="13" t="s">
+      <c r="G6" s="13"/>
+      <c r="I6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="9" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="10" t="s">
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -782,7 +1876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -872,14 +1966,14 @@
       </c>
       <c r="Y8">
         <f>EXP(-1*$D$4*X8*$C$4)</f>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z8">
         <f xml:space="preserve"> (I8 + J8 * R8 * 1 * Y8 * SIN((PI()*2/12) * (B8 + (3-L8)) - $D$4 / X8))</f>
-        <v>-28.132812228259336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-17.00484441249812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -969,14 +2063,14 @@
       </c>
       <c r="Y9">
         <f t="shared" ref="Y9:Y72" si="12">EXP(-1*$D$4*X9*$C$4)</f>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z9">
         <f t="shared" ref="Z9:Z31" si="13" xml:space="preserve"> (I9 + J9 * R9 * 1 * Y9 * SIN((PI()*2/12) * (B9 + (3-L9)) - $D$4 / X9))</f>
-        <v>-29.486793363755382</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-19.653194628042449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2015</v>
       </c>
@@ -1066,14 +2160,14 @@
       </c>
       <c r="Y10">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z10">
         <f t="shared" si="13"/>
-        <v>-25.663419479092116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-19.372334909694636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -1163,14 +2257,14 @@
       </c>
       <c r="Y11">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z11">
         <f t="shared" si="13"/>
-        <v>-18.239627564883673</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-16.64175494242421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -1260,14 +2354,14 @@
       </c>
       <c r="Y12">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z12">
         <f t="shared" si="13"/>
-        <v>-9.1333775083333322</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-12.273176951774708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -1357,14 +2451,14 @@
       </c>
       <c r="Y13">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z13">
         <f t="shared" si="13"/>
-        <v>-0.46582495572141802</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-7.3202552866782762</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -1454,14 +2548,14 @@
       </c>
       <c r="Y14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z14">
         <f t="shared" si="13"/>
-        <v>9.5732715907701618</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-1.3832117038219316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -1551,14 +2645,14 @@
       </c>
       <c r="Y15">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z15">
         <f t="shared" si="13"/>
-        <v>12.805279991666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+        <v>2.2057837602874955</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2015</v>
       </c>
@@ -1648,14 +2742,14 @@
       </c>
       <c r="Y16">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z16">
         <f t="shared" si="13"/>
-        <v>9.8660572115926719</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+        <v>2.6351590199703221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -1745,14 +2839,14 @@
       </c>
       <c r="Y17">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z17">
         <f t="shared" si="13"/>
-        <v>1.8359512416666739</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-8.8835579201980153E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -1842,14 +2936,14 @@
       </c>
       <c r="Y18">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z18">
         <f t="shared" si="13"/>
-        <v>-9.1333775083333304</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-5.5253529493632865</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2015</v>
       </c>
@@ -1939,14 +3033,14 @@
       </c>
       <c r="Y19" s="1">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z19" s="1">
         <f t="shared" si="13"/>
-        <v>-18.313946100658693</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-11.053815004516446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -2036,14 +3130,14 @@
       </c>
       <c r="Y20">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z20">
         <f t="shared" si="13"/>
-        <v>-21.620385034899037</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-13.878522650663767</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -2133,14 +3227,14 @@
       </c>
       <c r="Y21">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z21">
         <f t="shared" si="13"/>
-        <v>-21.520685955565448</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-14.835536336740057</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2016</v>
       </c>
@@ -2230,14 +3324,14 @@
       </c>
       <c r="Y22">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z22">
         <f t="shared" si="13"/>
-        <v>-19.522001367597902</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-15.038584042011522</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -2327,14 +3421,14 @@
       </c>
       <c r="Y23">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z23">
         <f t="shared" si="13"/>
-        <v>-14.524832497050141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-13.341026622018919</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2016</v>
       </c>
@@ -2424,14 +3518,14 @@
       </c>
       <c r="Y24">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z24">
         <f t="shared" si="13"/>
-        <v>-7.864075175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-10.138726960643753</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2016</v>
       </c>
@@ -2521,14 +3615,14 @@
       </c>
       <c r="Y25">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z25">
         <f t="shared" si="13"/>
-        <v>-1.5153120589533557</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-6.4380188326888526</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2016</v>
       </c>
@@ -2618,14 +3712,14 @@
       </c>
       <c r="Y26">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z26">
         <f t="shared" si="13"/>
-        <v>10.385242333333331</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1.7313304593948766</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2016</v>
       </c>
@@ -2715,14 +3809,14 @@
       </c>
       <c r="Y27">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z27">
         <f t="shared" si="13"/>
-        <v>7.8897080454738058</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1.9860731600280639</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2016</v>
       </c>
@@ -2812,14 +3906,14 @@
       </c>
       <c r="Y28">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z28">
         <f t="shared" si="13"/>
-        <v>1.228208083333338</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-0.3432756136563011</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2016</v>
       </c>
@@ -2909,14 +4003,14 @@
       </c>
       <c r="Y29">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z29">
         <f t="shared" si="13"/>
-        <v>-7.8639010833333325</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-4.6821558043398168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2016</v>
       </c>
@@ -3006,14 +4100,14 @@
       </c>
       <c r="Y30">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z30">
         <f t="shared" si="13"/>
-        <v>-15.534834317381794</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-9.3622348903929691</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2016</v>
       </c>
@@ -3103,14 +4197,14 @@
       </c>
       <c r="Y31">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z31">
         <f t="shared" si="13"/>
-        <v>-20.521257405020489</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-12.997688535326821</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2017</v>
       </c>
@@ -3200,14 +4294,14 @@
       </c>
       <c r="Y32">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z32">
         <f t="shared" ref="Z32:Z77" si="31" xml:space="preserve"> (I32 + J32 * R32 * 1 * Y32 * SIN((PI()*2/12) * (B32 + (3-L32)) - $D$4 / X32))</f>
-        <v>-20.894481789808736</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-14.419019321604416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2017</v>
       </c>
@@ -3297,14 +4391,14 @@
       </c>
       <c r="Y33">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z33">
         <f t="shared" si="31"/>
-        <v>-19.315967306653487</v>
-      </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-14.940728439664976</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2017</v>
       </c>
@@ -3394,14 +4488,14 @@
       </c>
       <c r="Y34">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z34">
         <f t="shared" si="31"/>
-        <v>-14.484415368280608</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-13.328791322693094</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2017</v>
       </c>
@@ -3491,14 +4585,14 @@
       </c>
       <c r="Y35">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z35">
         <f t="shared" si="31"/>
-        <v>-7.9343755833333338</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-10.221991319342143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2017</v>
       </c>
@@ -3588,14 +4682,14 @@
       </c>
       <c r="Y36">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z36">
         <f t="shared" si="31"/>
-        <v>-1.9443527370741815</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-6.6156957336758797</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2017</v>
       </c>
@@ -3685,14 +4779,14 @@
       </c>
       <c r="Y37">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z37">
         <f t="shared" si="31"/>
-        <v>1.4627956099378041</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-3.9701887941571483</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2017</v>
       </c>
@@ -3782,14 +4876,14 @@
       </c>
       <c r="Y38">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z38">
         <f t="shared" si="31"/>
-        <v>9.6838022499999994</v>
-      </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1.2275777629489788</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -3879,14 +4973,14 @@
       </c>
       <c r="Y39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z39">
         <f t="shared" si="31"/>
-        <v>7.0294109310073267</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1.2606369235832293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2017</v>
       </c>
@@ -3976,14 +5070,14 @@
       </c>
       <c r="Y40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z40">
         <f t="shared" si="31"/>
-        <v>0.755228750000005</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-0.78035644119023306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2017</v>
       </c>
@@ -4073,14 +5167,14 @@
       </c>
       <c r="Y41">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z41">
         <f t="shared" si="31"/>
-        <v>-7.9063421666666667</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-4.7972797297344254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2017</v>
       </c>
@@ -4170,14 +5264,14 @@
       </c>
       <c r="Y42">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z42">
         <f t="shared" si="31"/>
-        <v>-15.334965506522108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-9.4268461551629184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2017</v>
       </c>
@@ -4267,14 +5361,14 @@
       </c>
       <c r="Y43">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z43">
         <f t="shared" si="31"/>
-        <v>-18.729986271240438</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-12.271059639315581</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2018</v>
       </c>
@@ -4364,14 +5458,14 @@
       </c>
       <c r="Y44">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z44">
         <f t="shared" si="31"/>
-        <v>-20.065523260565733</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-14.177187763744948</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2018</v>
       </c>
@@ -4461,14 +5555,14 @@
       </c>
       <c r="Y45">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z45">
         <f t="shared" si="31"/>
-        <v>-18.11252026912312</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-14.24919371744225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2018</v>
       </c>
@@ -4558,14 +5652,14 @@
       </c>
       <c r="Y46">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z46">
         <f t="shared" si="31"/>
-        <v>-13.69476534873931</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-12.714879701320793</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2018</v>
       </c>
@@ -4655,14 +5749,14 @@
       </c>
       <c r="Y47">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z47">
         <f t="shared" si="31"/>
-        <v>-8.5198013333333353</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-10.463351517901863</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2018</v>
       </c>
@@ -4752,14 +5846,14 @@
       </c>
       <c r="Y48">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z48">
         <f t="shared" si="31"/>
-        <v>-3.4660487260775321</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-7.703932337651878</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2018</v>
       </c>
@@ -4849,14 +5943,14 @@
       </c>
       <c r="Y49">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z49">
         <f t="shared" si="31"/>
-        <v>-0.28423478008024006</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-5.4357495933556335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2018</v>
       </c>
@@ -4946,14 +6040,14 @@
       </c>
       <c r="Y50">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z50">
         <f t="shared" si="31"/>
-        <v>-2.2286597353219948</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-6.6122951549214566</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2018</v>
       </c>
@@ -5043,14 +6137,14 @@
       </c>
       <c r="Y51">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z51">
         <f t="shared" si="31"/>
-        <v>6.5670058000000004</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-1.2150207276110425</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2018</v>
       </c>
@@ -5140,14 +6234,14 @@
       </c>
       <c r="Y52">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z52">
         <f t="shared" si="31"/>
-        <v>4.2648903771281219</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-1.0439507524222424</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2018</v>
       </c>
@@ -5237,14 +6331,14 @@
       </c>
       <c r="Y53">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z53">
         <f t="shared" si="31"/>
-        <v>-1.9173226166666613</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-3.3304786547481999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2018</v>
       </c>
@@ -5334,14 +6428,14 @@
       </c>
       <c r="Y54">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z54">
         <f t="shared" si="31"/>
-        <v>-10.484638366666665</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-7.9560035802502878</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2018</v>
       </c>
@@ -5431,14 +6525,14 @@
       </c>
       <c r="Y55">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z55">
         <f t="shared" si="31"/>
-        <v>-17.946155920280503</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-12.277575704785537</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2019</v>
       </c>
@@ -5528,14 +6622,14 @@
       </c>
       <c r="Y56">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z56">
         <f t="shared" si="31"/>
-        <v>-22.506987393734434</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-15.566715023772886</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2019</v>
       </c>
@@ -5625,14 +6719,14 @@
       </c>
       <c r="Y57">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z57">
         <f t="shared" si="31"/>
-        <v>-26.773829557522134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-19.289690681967105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2019</v>
       </c>
@@ -5722,14 +6816,14 @@
       </c>
       <c r="Y58">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z58">
         <f t="shared" si="31"/>
-        <v>-24.851789428429278</v>
-      </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-19.817454940879045</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2019</v>
       </c>
@@ -5819,14 +6913,14 @@
       </c>
       <c r="Y59">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z59">
         <f t="shared" si="31"/>
-        <v>-18.533749104892209</v>
-      </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-17.260571242706892</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2019</v>
       </c>
@@ -5916,14 +7010,14 @@
       </c>
       <c r="Y60">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z60">
         <f t="shared" si="31"/>
-        <v>-11.102232199999998</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-13.370247099252412</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2019</v>
       </c>
@@ -6013,14 +7107,14 @@
       </c>
       <c r="Y61">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z61">
         <f t="shared" si="31"/>
-        <v>-4.7651535211244784</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-9.7143354986101258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2019</v>
       </c>
@@ -6110,14 +7204,14 @@
       </c>
       <c r="Y62">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z62">
         <f t="shared" si="31"/>
-        <v>2.4402566277869777</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-5.2966988264993455</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2019</v>
       </c>
@@ -6207,14 +7301,14 @@
       </c>
       <c r="Y63">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z63">
         <f t="shared" si="31"/>
-        <v>10.056026575000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9.5153076727786612E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2019</v>
       </c>
@@ -6304,14 +7398,14 @@
       </c>
       <c r="Y64">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z64">
         <f t="shared" si="31"/>
-        <v>7.4442877396036593</v>
-      </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+        <v>0.64905326870430713</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2019</v>
       </c>
@@ -6401,14 +7495,14 @@
       </c>
       <c r="Y65">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z65">
         <f t="shared" si="31"/>
-        <v>0.27329615833334131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-1.5355216963355431</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2019</v>
       </c>
@@ -6498,14 +7592,14 @@
       </c>
       <c r="Y66">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z66">
         <f t="shared" si="31"/>
-        <v>-10.076159008333331</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-6.7635503122237211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2019</v>
       </c>
@@ -6595,14 +7689,14 @@
       </c>
       <c r="Y67">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z67">
         <f t="shared" si="31"/>
-        <v>-18.159850981471592</v>
-      </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-11.782183026125237</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2020</v>
       </c>
@@ -6692,14 +7786,14 @@
       </c>
       <c r="Y68">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z68">
         <f t="shared" si="31"/>
-        <v>-24.129317588630332</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-16.289407928830634</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2020</v>
       </c>
@@ -6789,14 +7883,14 @@
       </c>
       <c r="Y69">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z69">
         <f t="shared" si="31"/>
-        <v>-25.388628495336214</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-18.091296657176922</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2020</v>
       </c>
@@ -6886,14 +7980,14 @@
       </c>
       <c r="Y70">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z70">
         <f t="shared" si="31"/>
-        <v>-23.379907986858058</v>
-      </c>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-18.483055200010259</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2020</v>
       </c>
@@ -6983,14 +8077,14 @@
       </c>
       <c r="Y71">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z71">
         <f t="shared" si="31"/>
-        <v>-18.109618902945069</v>
-      </c>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-16.88394658860447</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2020</v>
       </c>
@@ -7080,14 +8174,14 @@
       </c>
       <c r="Y72">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z72">
         <f t="shared" si="31"/>
-        <v>-11.27481334166667</v>
-      </c>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-13.535420942447086</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2020</v>
       </c>
@@ -7177,208 +8271,208 @@
       </c>
       <c r="Y73">
         <f t="shared" ref="Y73:Y80" si="37">EXP(-1*$D$4*X73*$C$4)</f>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z73">
         <f t="shared" si="31"/>
-        <v>-5.5563981988906637</v>
-      </c>
-    </row>
-    <row r="74" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15">
+        <v>-10.157010569821558</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="9">
         <v>2020</v>
       </c>
-      <c r="B74" s="15">
+      <c r="B74" s="9">
         <v>7</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C74" s="9">
         <v>8.5077569999999998</v>
       </c>
-      <c r="D74" s="15">
+      <c r="D74" s="9">
         <v>0</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="9">
         <v>0.45118429999999998</v>
       </c>
-      <c r="F74" s="15">
+      <c r="F74" s="9">
         <f t="shared" ref="F74:F91" si="38">IF(C74&lt;0,IF(C73&lt;0,F73+30,30),IF(D73&gt;0,IF(F73&gt;0,F73+30,30),0))</f>
         <v>300</v>
       </c>
-      <c r="G74" s="15">
+      <c r="G74" s="9">
         <f t="shared" ref="G74:G91" si="39">1000*(D73/1000)/(M74)</f>
         <v>0.32684792792792794</v>
       </c>
-      <c r="I74" s="15">
+      <c r="I74" s="9">
         <f t="shared" si="20"/>
         <v>-11.158579375000002</v>
       </c>
-      <c r="J74" s="15">
+      <c r="J74" s="9">
         <f t="shared" si="21"/>
         <v>20.526747</v>
       </c>
-      <c r="K74" s="15">
+      <c r="K74" s="9">
         <f t="shared" si="22"/>
         <v>9.5385939999999998</v>
       </c>
-      <c r="L74" s="15">
+      <c r="L74" s="9">
         <f t="shared" si="23"/>
         <v>8</v>
       </c>
-      <c r="M74" s="15">
+      <c r="M74" s="9">
         <f t="shared" si="24"/>
         <v>555</v>
       </c>
-      <c r="N74" s="15">
+      <c r="N74" s="9">
         <f t="shared" si="32"/>
         <v>77.079405027599989</v>
       </c>
-      <c r="O74" s="15">
+      <c r="O74" s="9">
         <f t="shared" si="25"/>
         <v>1159.95</v>
       </c>
-      <c r="P74" s="15">
+      <c r="P74" s="9">
         <f t="shared" si="26"/>
         <v>0.76910448155092881</v>
       </c>
-      <c r="Q74" s="15">
+      <c r="Q74" s="9">
         <f t="shared" si="33"/>
         <v>1.713990291638501</v>
       </c>
-      <c r="R74" s="15">
+      <c r="R74" s="9">
         <f t="shared" si="27"/>
         <v>0.5710867380701794</v>
       </c>
-      <c r="S74" s="15">
+      <c r="S74" s="9">
         <f t="shared" si="28"/>
         <v>0.33299999999999996</v>
       </c>
-      <c r="T74" s="15">
+      <c r="T74" s="9">
         <f t="shared" si="34"/>
         <v>1.4679402270902751</v>
       </c>
-      <c r="U74" s="15">
+      <c r="U74" s="9">
         <f t="shared" si="29"/>
         <v>152.45820193827439</v>
       </c>
-      <c r="V74" s="15">
+      <c r="V74" s="9">
         <f t="shared" si="30"/>
         <v>5.160277254533617E-2</v>
       </c>
-      <c r="W74" s="15">
+      <c r="W74" s="9">
         <f t="shared" si="35"/>
         <v>0.59725431186731681</v>
       </c>
-      <c r="X74" s="15">
+      <c r="X74" s="9">
         <f t="shared" si="36"/>
         <v>1.5104116738158395</v>
       </c>
-      <c r="Y74" s="15">
+      <c r="Y74" s="9">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="Z74" s="15">
+        <v>0.54653076982131776</v>
+      </c>
+      <c r="Z74" s="9">
         <f t="shared" si="31"/>
-        <v>-1.0065506906835253</v>
-      </c>
-    </row>
-    <row r="75" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="15">
+        <v>-6.952593303481768</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="9">
         <v>2020</v>
       </c>
-      <c r="B75" s="15">
+      <c r="B75" s="9">
         <v>8</v>
       </c>
-      <c r="C75" s="15">
+      <c r="C75" s="9">
         <v>5.0305869999999997</v>
       </c>
-      <c r="D75" s="15">
+      <c r="D75" s="9">
         <v>0</v>
       </c>
-      <c r="E75" s="15">
+      <c r="E75" s="9">
         <v>0.45118429999999998</v>
       </c>
-      <c r="F75" s="15">
+      <c r="F75" s="9">
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="G75" s="15">
+      <c r="G75" s="9">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="I75" s="15">
+      <c r="I75" s="9">
         <f t="shared" si="20"/>
         <v>-11.534246625000002</v>
       </c>
-      <c r="J75" s="15">
+      <c r="J75" s="9">
         <f t="shared" si="21"/>
         <v>20.011328500000001</v>
       </c>
-      <c r="K75" s="15">
+      <c r="K75" s="9">
         <f t="shared" si="22"/>
         <v>8.5077569999999998</v>
       </c>
-      <c r="L75" s="15">
+      <c r="L75" s="9">
         <f t="shared" si="23"/>
         <v>7</v>
       </c>
-      <c r="M75" s="15">
+      <c r="M75" s="9">
         <f t="shared" si="24"/>
         <v>165</v>
       </c>
-      <c r="N75" s="15">
+      <c r="N75" s="9">
         <f t="shared" si="32"/>
         <v>10.3843158084</v>
       </c>
-      <c r="O75" s="15">
+      <c r="O75" s="9">
         <f t="shared" si="25"/>
         <v>344.85</v>
       </c>
-      <c r="P75" s="15">
+      <c r="P75" s="9">
         <f t="shared" si="26"/>
         <v>0.3485249829636074</v>
       </c>
-      <c r="Q75" s="15">
+      <c r="Q75" s="9">
         <f t="shared" si="33"/>
         <v>1.1538056040391906</v>
       </c>
-      <c r="R75" s="15">
+      <c r="R75" s="9">
         <f t="shared" si="27"/>
         <v>1</v>
       </c>
-      <c r="S75" s="15">
+      <c r="S75" s="9">
         <f t="shared" si="28"/>
         <v>0.33299999999999996</v>
       </c>
-      <c r="T75" s="15">
+      <c r="T75" s="9">
         <f t="shared" si="34"/>
         <v>1.4679402270902751</v>
       </c>
-      <c r="U75" s="15">
+      <c r="U75" s="9">
         <f t="shared" si="29"/>
         <v>152.45820193827439</v>
       </c>
-      <c r="V75" s="15">
+      <c r="V75" s="9">
         <f t="shared" si="30"/>
         <v>5.160277254533617E-2</v>
       </c>
-      <c r="W75" s="15">
+      <c r="W75" s="9">
         <f t="shared" si="35"/>
         <v>0.59725431186731681</v>
       </c>
-      <c r="X75" s="15">
+      <c r="X75" s="9">
         <f t="shared" si="36"/>
         <v>1.5104116738158395</v>
       </c>
-      <c r="Y75" s="15">
+      <c r="Y75" s="9">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="Z75" s="15">
+        <v>0.54653076982131776</v>
+      </c>
+      <c r="Z75" s="9">
         <f t="shared" si="31"/>
-        <v>5.7960722194755441</v>
-      </c>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-0.79958565351010868</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2020</v>
       </c>
@@ -7468,14 +8562,14 @@
       </c>
       <c r="Y76">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z76">
         <f t="shared" si="31"/>
-        <v>-1.6098154583333262</v>
-      </c>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-3.3655081831444633</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2020</v>
       </c>
@@ -7565,14 +8659,14 @@
       </c>
       <c r="Y77">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z77">
         <f t="shared" si="31"/>
-        <v>-11.630236208333335</v>
-      </c>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-8.0755273371996079</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2020</v>
       </c>
@@ -7662,14 +8756,14 @@
       </c>
       <c r="Y78">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z78">
         <f t="shared" ref="Z78:Z80" si="50" xml:space="preserve"> (I78 + J78 * R78 * 1 * Y78 * SIN((PI()*2/12) * (B78 + (3-L78)) - $D$4 / X78))</f>
-        <v>-20.784232991948862</v>
-      </c>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-13.515461036540215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2020</v>
       </c>
@@ -7759,14 +8853,14 @@
       </c>
       <c r="Y79">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z79">
         <f t="shared" si="50"/>
-        <v>-26.166378925642665</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+        <v>-17.376210661868939</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2021</v>
       </c>
@@ -7856,14 +8950,14 @@
       </c>
       <c r="Y80">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0.54653076982131776</v>
       </c>
       <c r="Z80">
         <f t="shared" si="50"/>
-        <v>-25.379169742365068</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+        <v>-18.158592383685601</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>2</v>
       </c>
@@ -7876,7 +8970,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>3</v>
       </c>
@@ -7889,7 +8983,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>4</v>
       </c>
@@ -7902,7 +8996,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>5</v>
       </c>
@@ -7915,7 +9009,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>6</v>
       </c>
@@ -7928,7 +9022,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>7</v>
       </c>
@@ -7941,7 +9035,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>8</v>
       </c>
@@ -7954,7 +9048,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>9</v>
       </c>
@@ -7967,7 +9061,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B89">
         <v>10</v>
       </c>
@@ -7980,7 +9074,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B90">
         <v>11</v>
       </c>
@@ -7993,7 +9087,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B91">
         <v>12</v>
       </c>
@@ -8017,6 +9111,7 @@
     <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8028,12 +9123,12 @@
       <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="7" width="10.42578125" customWidth="1"/>
+    <col min="5" max="7" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -8056,7 +9151,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.45</v>
       </c>
@@ -8082,17 +9177,17 @@
         <v>2951.8</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="M3" s="14" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="M3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -8169,7 +9264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2000</v>
       </c>
@@ -8281,27 +9376,27 @@
       <selection pane="bottomRight" activeCell="F8" sqref="F8:F91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="5" max="7" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="F2" s="10" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -8324,7 +9419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.45118429999999998</v>
       </c>
@@ -8350,42 +9445,42 @@
         <v>2954.4575691999999</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="I6" s="13" t="s">
+      <c r="G6" s="13"/>
+      <c r="I6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="9" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="10" t="s">
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -8462,7 +9557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -8559,7 +9654,7 @@
         <v>-21.651138732139415</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -8656,7 +9751,7 @@
         <v>-23.974551472604432</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2015</v>
       </c>
@@ -8753,7 +9848,7 @@
         <v>-22.349114732611667</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -8850,7 +9945,7 @@
         <v>-17.694591810981233</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -8947,7 +10042,7 @@
         <v>-11.286362303499557</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -9044,7 +10139,7 @@
         <v>-4.6418502568594722</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -9141,7 +10236,7 @@
         <v>3.1914821610188024</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -9238,7 +10333,7 @@
         <v>6.8637128480416045</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2015</v>
       </c>
@@ -9335,7 +10430,7 @@
         <v>6.0566345383720996</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -9432,7 +10527,7 @@
         <v>1.1794047677688493</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -9529,7 +10624,7 @@
         <v>-6.6593271251869819</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2015</v>
       </c>
@@ -9626,7 +10721,7 @@
         <v>-13.890749761476293</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -9723,7 +10818,7 @@
         <v>-17.111006048788724</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -9820,7 +10915,7 @@
         <v>-17.773313018364803</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2016</v>
       </c>
@@ -9917,7 +11012,7 @@
         <v>-17.160022100155505</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -10014,7 +11109,7 @@
         <v>-14.121035274103386</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2016</v>
       </c>
@@ -10111,7 +11206,7 @@
         <v>-9.4238215209070582</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2016</v>
       </c>
@@ -10208,7 +11303,7 @@
         <v>-4.5144450349439911</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2016</v>
       </c>
@@ -10305,7 +11400,7 @@
         <v>5.5342760862960239</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2016</v>
       </c>
@@ -10402,7 +11497,7 @@
         <v>4.7795217323697168</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2016</v>
       </c>
@@ -10499,7 +11594,7 @@
         <v>0.69217361506903696</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2016</v>
       </c>
@@ -10596,7 +11691,7 @@
         <v>-5.6821537038711769</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2016</v>
       </c>
@@ -10693,7 +11788,7 @@
         <v>-11.774210875856902</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2016</v>
       </c>
@@ -10790,7 +11885,7 @@
         <v>-16.139027176976779</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2017</v>
       </c>
@@ -10887,7 +11982,7 @@
         <v>-17.264649371268042</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2017</v>
       </c>
@@ -10984,7 +12079,7 @@
         <v>-17.010979226476628</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2017</v>
       </c>
@@ -11081,7 +12176,7 @@
         <v>-14.090230992091037</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2017</v>
       </c>
@@ -11178,7 +12273,7 @@
         <v>-9.5030114104075913</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2017</v>
       </c>
@@ -11275,7 +12370,7 @@
         <v>-4.7903436658899299</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2017</v>
       </c>
@@ -11372,7 +12467,7 @@
         <v>-1.701738256432499</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2017</v>
       </c>
@@ -11469,7 +12564,7 @@
         <v>4.9436500319504315</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -11566,7 +12661,7 @@
         <v>3.9902727882482871</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2017</v>
       </c>
@@ -11663,7 +12758,7 @@
         <v>0.23143929357039728</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2017</v>
       </c>
@@ -11760,7 +12855,7 @@
         <v>-5.774433974912589</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2017</v>
       </c>
@@ -11857,7 +12952,7 @@
         <v>-11.735475147419557</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2017</v>
       </c>
@@ -11954,7 +13049,7 @@
         <v>-14.967874962450077</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2018</v>
       </c>
@@ -12051,7 +13146,7 @@
         <v>-16.764805947701586</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2018</v>
       </c>
@@ -12148,7 +13243,7 @@
         <v>-16.077220729561191</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2018</v>
       </c>
@@ -12245,7 +13340,7 @@
         <v>-13.360525494402935</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2018</v>
       </c>
@@ -12342,7 +13437,7 @@
         <v>-9.8525087471012025</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2018</v>
       </c>
@@ -12439,7 +13534,7 @@
         <v>-6.0479568250314326</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2018</v>
       </c>
@@ -12536,7 +13631,7 @@
         <v>-3.2848219117920499</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2018</v>
       </c>
@@ -12633,7 +13728,7 @@
         <v>-4.7819824970599374</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2018</v>
       </c>
@@ -12730,7 +13825,7 @@
         <v>2.2047764904230753</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2018</v>
       </c>
@@ -12827,7 +13922,7 @@
         <v>1.4680566738316276</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2018</v>
       </c>
@@ -12924,7 +14019,7 @@
         <v>-2.3993513815202867</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2018</v>
       </c>
@@ -13021,7 +14116,7 @@
         <v>-8.7507339101081811</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2018</v>
       </c>
@@ -13118,7 +14213,7 @@
         <v>-14.492603508415369</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2019</v>
       </c>
@@ -13215,7 +14310,7 @@
         <v>-18.464508100029185</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2019</v>
       </c>
@@ -13312,7 +14407,7 @@
         <v>-22.57858172020687</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2019</v>
       </c>
@@ -13409,7 +14504,7 @@
         <v>-22.199572866499331</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2019</v>
       </c>
@@ -13506,7 +14601,7 @@
         <v>-18.099467018689388</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2019</v>
       </c>
@@ -13603,7 +14698,7 @@
         <v>-12.657427581507834</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2019</v>
       </c>
@@ -13700,7 +14795,7 @@
         <v>-7.7804163744900539</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2019</v>
       </c>
@@ -13797,7 +14892,7 @@
         <v>-2.0662642337920669</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2019</v>
       </c>
@@ -13894,7 +14989,7 @@
         <v>4.4724405811740375</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2019</v>
       </c>
@@ -13991,7 +15086,7 @@
         <v>3.864383891242861</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2019</v>
       </c>
@@ -14088,7 +15183,7 @@
         <v>-0.34369319941295373</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2019</v>
       </c>
@@ -14185,7 +15280,7 @@
         <v>-7.8046775702570246</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2019</v>
       </c>
@@ -14282,7 +15377,7 @@
         <v>-14.274290627389497</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2020</v>
       </c>
@@ -14379,7 +15474,7 @@
         <v>-19.562829304765526</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2020</v>
       </c>
@@ -14476,7 +15571,7 @@
         <v>-21.298095687052477</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2020</v>
       </c>
@@ -14573,7 +15668,7 @@
         <v>-20.800120311897579</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2020</v>
       </c>
@@ -14670,7 +15765,7 @@
         <v>-17.691541000805579</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2020</v>
       </c>
@@ -14743,11 +15838,11 @@
         <v>1.4679402270902751</v>
       </c>
       <c r="U72">
-        <f t="shared" ref="U72:U116" si="21">($G$4 * (1 - $A$4) * $F$4 + T72 * ($A$4 - E72) * 2.25 + E72 * 51.51) / ($G$4 * (1 - $A$4) + T72 * ($A$4 - E72) + E72)</f>
+        <f t="shared" ref="U72:U76" si="21">($G$4 * (1 - $A$4) * $F$4 + T72 * ($A$4 - E72) * 2.25 + E72 * 51.51) / ($G$4 * (1 - $A$4) + T72 * ($A$4 - E72) + E72)</f>
         <v>152.45820193827439</v>
       </c>
       <c r="V72">
-        <f t="shared" ref="V72:V120" si="22">U72/$H$4</f>
+        <f t="shared" ref="V72:V80" si="22">U72/$H$4</f>
         <v>5.160277254533617E-2</v>
       </c>
       <c r="W72">
@@ -14767,7 +15862,7 @@
         <v>-12.824929481244967</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2020</v>
       </c>
@@ -14808,7 +15903,7 @@
         <v>8</v>
       </c>
       <c r="M73">
-        <f t="shared" ref="M73:M118" si="23">(165+(1.3*F73))</f>
+        <f t="shared" ref="M73:M80" si="23">(165+(1.3*F73))</f>
         <v>516</v>
       </c>
       <c r="N73">
@@ -14816,11 +15911,11 @@
         <v>67.447117062144002</v>
       </c>
       <c r="O73">
-        <f t="shared" ref="O73:O118" si="25">2090 * M73 / 1000</f>
+        <f t="shared" ref="O73:O80" si="25">2090 * M73 / 1000</f>
         <v>1078.44</v>
       </c>
       <c r="P73">
-        <f t="shared" ref="P73:P118" si="26">1000000 / 86400 * (N73 / O73)</f>
+        <f t="shared" ref="P73:P80" si="26">1000000 / 86400 * (N73 / O73)</f>
         <v>0.72385847053150854</v>
       </c>
       <c r="Q73">
@@ -14828,11 +15923,11 @@
         <v>1.662809576715472</v>
       </c>
       <c r="R73">
-        <f t="shared" ref="R73:R118" si="28">IF(G73&gt;0,EXP(-1 * G73 * Q73),1)</f>
+        <f t="shared" ref="R73:R80" si="28">IF(G73&gt;0,EXP(-1 * G73 * Q73),1)</f>
         <v>0.56682712652352307</v>
       </c>
       <c r="S73">
-        <f t="shared" ref="S73:S118" si="29">0.035+0.298*(E73/$A$4)</f>
+        <f t="shared" ref="S73:S80" si="29">0.035+0.298*(E73/$A$4)</f>
         <v>0.33299999999999996</v>
       </c>
       <c r="T73">
@@ -14860,11 +15955,11 @@
         <v>0.73927719417098059</v>
       </c>
       <c r="Z73">
-        <f t="shared" ref="Z73:Z118" si="34" xml:space="preserve"> (I73 + J73 * R73 * 1 * Y73 * SIN((PI()*2/12) * (B73 + (3-L73)) - $D$4 / X73))</f>
+        <f t="shared" ref="Z73:Z80" si="34" xml:space="preserve"> (I73 + J73 * R73 * 1 * Y73 * SIN((PI()*2/12) * (B73 + (3-L73)) - $D$4 / X73))</f>
         <v>-8.3592968693997527</v>
       </c>
     </row>
-    <row r="74" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
         <v>2020</v>
       </c>
@@ -14961,7 +16056,7 @@
         <v>-4.4699240080997606</v>
       </c>
     </row>
-    <row r="75" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <v>2020</v>
       </c>
@@ -15058,7 +16153,7 @@
         <v>2.3213104429554914</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2020</v>
       </c>
@@ -15155,7 +16250,7 @@
         <v>-2.2086837876595879</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2020</v>
       </c>
@@ -15252,7 +16347,7 @@
         <v>-9.1927448052502498</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2020</v>
       </c>
@@ -15349,7 +16444,7 @@
         <v>-16.355772255117383</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2020</v>
       </c>
@@ -15446,7 +16541,7 @@
         <v>-21.046396409064975</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2021</v>
       </c>
@@ -15543,7 +16638,7 @@
         <v>-21.331661798985124</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>2</v>
       </c>
@@ -15556,7 +16651,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>3</v>
       </c>
@@ -15569,7 +16664,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>4</v>
       </c>
@@ -15582,7 +16677,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>5</v>
       </c>
@@ -15595,7 +16690,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>6</v>
       </c>
@@ -15608,7 +16703,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>7</v>
       </c>
@@ -15621,7 +16716,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>8</v>
       </c>
@@ -15634,7 +16729,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>9</v>
       </c>
@@ -15647,7 +16742,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B89">
         <v>10</v>
       </c>
@@ -15660,7 +16755,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B90">
         <v>11</v>
       </c>
@@ -15673,7 +16768,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B91">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Compile v5-rc6 Add reference docs
</commit_message>
<xml_diff>
--- a/deploy/docs/Soil_temp_calculations.xlsx
+++ b/deploy/docs/Soil_temp_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\aruzicka555\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC813EA-1DB2-48FA-8257-64FCE6C71A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C248C9A-60AB-4CCF-A04F-1FC4A98EF42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14895" yWindow="-7410" windowWidth="14160" windowHeight="13440" activeTab="3" xr2:uid="{B5CA6E75-4B5B-4C46-9481-06C855E228A5}"/>
   </bookViews>
@@ -885,7 +885,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1143,7 +1145,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1399,9 +1403,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -18448,7 +18452,7 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18539,7 +18543,7 @@
         <v>-4</v>
       </c>
       <c r="K2">
-        <f>IF(I2 &gt;= 12,(B2 + (I2-5-12)),(B2 + (I2-5)))</f>
+        <f>IF(I2 &gt;= 9,(B2 + (I2-5-12)),(B2 + (I2-5)))</f>
         <v>-3</v>
       </c>
       <c r="L2">
@@ -18598,7 +18602,7 @@
         <v>-3</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K66" si="1">IF(I3 &gt;= 12,(B3 + (I3-5-12)),(B3 + (I3-5)))</f>
+        <f t="shared" ref="K3:K66" si="1">IF(I3 &gt;= 9,(B3 + (I3-5-12)),(B3 + (I3-5)))</f>
         <v>-2</v>
       </c>
       <c r="L3">
@@ -22374,7 +22378,7 @@
         <v>1</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K73" si="7">IF(I67 &gt;= 12,(B67 + (I67-5-12)),(B67 + (I67-5)))</f>
+        <f t="shared" ref="K67:K73" si="7">IF(I67 &gt;= 9,(B67 + (I67-5-12)),(B67 + (I67-5)))</f>
         <v>2</v>
       </c>
       <c r="L67">

</xml_diff>